<commit_message>
made some small CSS updates
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scratch\portfolio_v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scratch\projects\portfolio_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="101">
   <si>
     <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (</t>
   </si>
@@ -32,42 +33,6 @@
     <t>).JPEG</t>
   </si>
   <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (10).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (11).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (12).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (13).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (14).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (15).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (16).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (17).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (18).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (19).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (20).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (21).JPEG</t>
-  </si>
-  <si>
     <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (22).JPEG</t>
   </si>
   <si>
@@ -254,28 +219,115 @@
     <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (1).JPEG</t>
   </si>
   <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (2).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (3).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (4).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (5).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (6).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (7).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (8).JPEG</t>
-  </si>
-  <si>
-    <t>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (9).JPEG</t>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (1).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (2).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (3).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (4).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (5).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (6).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (7).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (8).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (9).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (10).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (11).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (12).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (13).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (14).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (15).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (16).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (17).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (18).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (19).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (20).JPEG</t>
+  </si>
+  <si>
+    <t>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (21).JPEG</t>
+  </si>
+  <si>
+    <t>ProjectName</t>
+  </si>
+  <si>
+    <t>ProjectUrl</t>
+  </si>
+  <si>
+    <t>ProjectDesc</t>
+  </si>
+  <si>
+    <t>SocialMedia</t>
+  </si>
+  <si>
+    <t>Starting Video Call</t>
+  </si>
+  <si>
+    <t>CryptoTracker</t>
+  </si>
+  <si>
+    <t>Clicking on a coin</t>
+  </si>
+  <si>
+    <t>Shows week price range of selected coin</t>
+  </si>
+  <si>
+    <t>Shows day price range of selected coin</t>
+  </si>
+  <si>
+    <t>Shows month price range of selected coin</t>
+  </si>
+  <si>
+    <t>Shows year price range of selected coin</t>
+  </si>
+  <si>
+    <t>Selecting different fiat currency</t>
+  </si>
+  <si>
+    <t>Price is recalculated in EUR now</t>
+  </si>
+  <si>
+    <t>Searching for coins</t>
+  </si>
+  <si>
+    <t>Toggling Day/Night mode</t>
   </si>
 </sst>
 </file>
@@ -311,12 +363,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -332,13 +390,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -624,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8:Q9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +700,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -647,28 +710,28 @@
       </c>
       <c r="D1" t="str">
         <f>CONCATENATE(A1,B1,C1)</f>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (1).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (1).JPEG</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="O1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q1" t="str">
         <f>CONCATENATE(M1,N1,O1,N1,P1)</f>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (1).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (1).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (1).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (1).JPEG" },</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -678,28 +741,28 @@
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D65" si="0">CONCATENATE(A2,B2,C2)</f>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (2).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (2).JPEG</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="O2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q2" t="str">
         <f t="shared" ref="Q2:Q65" si="1">CONCATENATE(M2,N2,O2,N2,P2)</f>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (2).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (2).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (2).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (2).JPEG" },</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -709,28 +772,28 @@
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (3).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (3).JPEG</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="O3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P3" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q3" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (3).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (3).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (3).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (3).JPEG" },</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -740,28 +803,28 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (4).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (4).JPEG</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="O4" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (4).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (4).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (4).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (4).JPEG" },</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -771,28 +834,28 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (5).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (5).JPEG</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="O5" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (5).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (5).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (5).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (5).JPEG" },</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -802,28 +865,28 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (6).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (6).JPEG</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="O6" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P6" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (6).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (6).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (6).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (6).JPEG" },</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -833,28 +896,28 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (7).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (7).JPEG</v>
       </c>
       <c r="M7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" t="s">
         <v>71</v>
       </c>
-      <c r="N7" t="s">
-        <v>81</v>
-      </c>
       <c r="O7" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P7" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (7).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (7).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (7).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (7).JPEG" },</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -864,28 +927,28 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (8).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (8).JPEG</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N8" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="O8" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P8" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (8).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (8).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (8).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (8).JPEG" },</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B9">
         <v>9</v>
@@ -895,28 +958,28 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (9).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (9).JPEG</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="O9" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P9" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (9).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (9).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (9).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (9).JPEG" },</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -926,28 +989,28 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (10).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (10).JPEG</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N10" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="O10" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P10" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (10).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (10).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (10).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (10).JPEG" },</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B11">
         <v>11</v>
@@ -957,28 +1020,28 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (11).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (11).JPEG</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N11" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="O11" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P11" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q11" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (11).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (11).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (11).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (11).JPEG" },</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B12">
         <v>12</v>
@@ -988,28 +1051,28 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (12).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (12).JPEG</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N12" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="O12" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P12" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (12).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (12).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (12).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (12).JPEG" },</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B13">
         <v>13</v>
@@ -1019,28 +1082,28 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (13).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (13).JPEG</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N13" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="O13" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P13" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (13).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (13).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (13).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (13).JPEG" },</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B14">
         <v>14</v>
@@ -1050,28 +1113,28 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (14).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (14).JPEG</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N14" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="O14" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P14" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (14).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (14).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (14).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (14).JPEG" },</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B15">
         <v>15</v>
@@ -1081,28 +1144,28 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (15).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (15).JPEG</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N15" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="O15" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P15" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (15).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (15).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (15).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (15).JPEG" },</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -1112,28 +1175,28 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (16).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (16).JPEG</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N16" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="O16" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P16" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (16).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (16).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (16).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (16).JPEG" },</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -1143,28 +1206,28 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (17).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (17).JPEG</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N17" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="O17" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P17" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (17).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (17).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (17).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (17).JPEG" },</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B18">
         <v>18</v>
@@ -1174,28 +1237,28 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (18).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (18).JPEG</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N18" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="O18" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P18" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q18" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (18).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (18).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (18).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (18).JPEG" },</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B19">
         <v>19</v>
@@ -1205,28 +1268,28 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (19).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (19).JPEG</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N19" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="O19" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (19).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (19).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (19).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (19).JPEG" },</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B20">
         <v>20</v>
@@ -1236,28 +1299,28 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (20).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (20).JPEG</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N20" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="O20" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P20" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (20).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (20).JPEG" },</v>
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (20).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (20).JPEG" },</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B21">
         <v>21</v>
@@ -1267,52 +1330,52 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (21).JPEG</v>
+        <v>https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (21).JPEG</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N21" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="O21" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P21" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q21" t="str">
         <f t="shared" si="1"/>
-        <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (21).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (21).JPEG" },</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22">
+        <v>{ original: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (21).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto (21).JPEG" },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="5">
         <v>22</v>
       </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="str">
+      <c r="C22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5" t="str">
         <f t="shared" si="0"/>
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (22).JPEG</v>
       </c>
-      <c r="M22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="N22" t="s">
-        <v>14</v>
-      </c>
-      <c r="O22" t="s">
-        <v>72</v>
-      </c>
-      <c r="P22" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q22" t="str">
+      <c r="M22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q22" s="5" t="str">
         <f t="shared" si="1"/>
         <v>{ original: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (22).JPEG", thumbnail: "https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (22).JPEG" },</v>
       </c>
@@ -1332,16 +1395,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (23).JPEG</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N23" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="O23" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P23" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q23" t="str">
         <f t="shared" si="1"/>
@@ -1363,16 +1426,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (24).JPEG</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N24" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O24" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P24" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="1"/>
@@ -1394,16 +1457,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (25).JPEG</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N25" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="O25" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P25" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q25" t="str">
         <f t="shared" si="1"/>
@@ -1425,16 +1488,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (26).JPEG</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N26" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="O26" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P26" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" si="1"/>
@@ -1443,7 +1506,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B27">
         <v>27</v>
@@ -1456,16 +1519,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid (27).JPEG</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N27" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="O27" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P27" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="1"/>
@@ -1487,16 +1550,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (28).JPEG</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N28" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="O28" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P28" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q28" t="str">
         <f t="shared" si="1"/>
@@ -1518,16 +1581,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (29).JPEG</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N29" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="O29" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P29" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q29" t="str">
         <f t="shared" si="1"/>
@@ -1549,16 +1612,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (30).JPEG</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N30" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="O30" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P30" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q30" t="str">
         <f t="shared" si="1"/>
@@ -1580,16 +1643,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (31).JPEG</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N31" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="O31" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P31" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" si="1"/>
@@ -1611,16 +1674,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (32).JPEG</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N32" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="O32" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P32" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" si="1"/>
@@ -1642,16 +1705,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (33).JPEG</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N33" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="O33" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P33" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" si="1"/>
@@ -1673,16 +1736,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (34).JPEG</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N34" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="O34" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P34" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" si="1"/>
@@ -1704,16 +1767,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (35).JPEG</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N35" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="O35" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P35" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" si="1"/>
@@ -1735,16 +1798,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (36).JPEG</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N36" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="O36" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P36" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" si="1"/>
@@ -1766,16 +1829,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (37).JPEG</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N37" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="O37" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P37" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" si="1"/>
@@ -1797,16 +1860,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (38).JPEG</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N38" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="O38" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P38" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" si="1"/>
@@ -1828,16 +1891,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (39).JPEG</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N39" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="O39" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P39" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" si="1"/>
@@ -1859,16 +1922,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (40).JPEG</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N40" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="O40" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P40" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" si="1"/>
@@ -1890,16 +1953,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (41).JPEG</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N41" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="O41" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P41" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" si="1"/>
@@ -1921,16 +1984,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (42).JPEG</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N42" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="O42" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P42" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" si="1"/>
@@ -1952,16 +2015,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (43).JPEG</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N43" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="O43" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P43" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" si="1"/>
@@ -1983,16 +2046,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (44).JPEG</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N44" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="O44" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P44" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" si="1"/>
@@ -2014,16 +2077,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (45).JPEG</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N45" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="O45" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P45" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" si="1"/>
@@ -2045,16 +2108,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (46).JPEG</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N46" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O46" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P46" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" si="1"/>
@@ -2076,16 +2139,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (47).JPEG</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N47" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="O47" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P47" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" si="1"/>
@@ -2107,16 +2170,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (48).JPEG</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N48" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="O48" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P48" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" si="1"/>
@@ -2138,16 +2201,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (49).JPEG</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N49" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="O49" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P49" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q49" t="str">
         <f t="shared" si="1"/>
@@ -2169,16 +2232,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (50).JPEG</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N50" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="O50" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P50" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q50" t="str">
         <f t="shared" si="1"/>
@@ -2200,16 +2263,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (51).JPEG</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N51" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="O51" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P51" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q51" t="str">
         <f t="shared" si="1"/>
@@ -2231,16 +2294,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (52).JPEG</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N52" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="O52" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P52" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q52" t="str">
         <f t="shared" si="1"/>
@@ -2262,16 +2325,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (53).JPEG</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N53" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="O53" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P53" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q53" t="str">
         <f t="shared" si="1"/>
@@ -2293,16 +2356,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (54).JPEG</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N54" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="O54" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P54" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q54" t="str">
         <f t="shared" si="1"/>
@@ -2324,16 +2387,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (55).JPEG</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N55" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="O55" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P55" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q55" t="str">
         <f t="shared" si="1"/>
@@ -2355,16 +2418,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (56).JPEG</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N56" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="O56" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P56" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q56" t="str">
         <f t="shared" si="1"/>
@@ -2386,16 +2449,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (57).JPEG</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N57" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="O57" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P57" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q57" t="str">
         <f t="shared" si="1"/>
@@ -2417,16 +2480,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (58).JPEG</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N58" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="O58" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P58" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q58" t="str">
         <f t="shared" si="1"/>
@@ -2448,16 +2511,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (59).JPEG</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N59" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="O59" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P59" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q59" t="str">
         <f t="shared" si="1"/>
@@ -2479,16 +2542,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (60).JPEG</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N60" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="O60" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P60" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q60" t="str">
         <f t="shared" si="1"/>
@@ -2510,16 +2573,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (61).JPEG</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N61" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="O61" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P61" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q61" t="str">
         <f t="shared" si="1"/>
@@ -2541,16 +2604,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (62).JPEG</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N62" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="O62" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P62" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q62" t="str">
         <f t="shared" si="1"/>
@@ -2572,16 +2635,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (63).JPEG</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N63" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="O63" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P63" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q63" t="str">
         <f t="shared" si="1"/>
@@ -2603,16 +2666,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (64).JPEG</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N64" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="O64" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P64" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q64" t="str">
         <f t="shared" si="1"/>
@@ -2634,16 +2697,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (65).JPEG</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N65" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="O65" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P65" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q65" t="str">
         <f t="shared" si="1"/>
@@ -2665,16 +2728,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (66).JPEG</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N66" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="O66" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P66" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q66" t="str">
         <f t="shared" ref="Q66:Q78" si="3">CONCATENATE(M66,N66,O66,N66,P66)</f>
@@ -2696,16 +2759,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (67).JPEG</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N67" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="O67" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P67" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q67" t="str">
         <f t="shared" si="3"/>
@@ -2727,16 +2790,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (68).JPEG</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N68" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="O68" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P68" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q68" t="str">
         <f t="shared" si="3"/>
@@ -2758,16 +2821,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (69).JPEG</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N69" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="O69" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P69" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q69" t="str">
         <f t="shared" si="3"/>
@@ -2789,16 +2852,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (70).JPEG</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N70" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="O70" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P70" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q70" t="str">
         <f t="shared" si="3"/>
@@ -2820,16 +2883,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (71).JPEG</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N71" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="O71" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P71" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q71" t="str">
         <f t="shared" si="3"/>
@@ -2851,16 +2914,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (72).JPEG</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N72" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="O72" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P72" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q72" t="str">
         <f t="shared" si="3"/>
@@ -2882,16 +2945,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (73).JPEG</v>
       </c>
       <c r="M73" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N73" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="O73" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P73" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q73" t="str">
         <f t="shared" si="3"/>
@@ -2913,16 +2976,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (74).JPEG</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N74" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="O74" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P74" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q74" t="str">
         <f t="shared" si="3"/>
@@ -2944,16 +3007,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (75).JPEG</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N75" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="O75" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P75" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q75" t="str">
         <f t="shared" si="3"/>
@@ -2975,16 +3038,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (76).JPEG</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N76" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="O76" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P76" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q76" t="str">
         <f t="shared" si="3"/>
@@ -3006,16 +3069,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (77).JPEG</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N77" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="O77" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P77" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q77" t="str">
         <f t="shared" si="3"/>
@@ -3037,16 +3100,16 @@
         <v>https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM (78).JPEG</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N78" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="O78" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="P78" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q78" t="str">
         <f t="shared" si="3"/>
@@ -3120,15 +3183,270 @@
   <hyperlinks>
     <hyperlink ref="A27" r:id="rId1"/>
     <hyperlink ref="A1" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
-    <hyperlink ref="A5" r:id="rId6"/>
-    <hyperlink ref="A6" r:id="rId7"/>
-    <hyperlink ref="A7" r:id="rId8"/>
-    <hyperlink ref="A8:A9" r:id="rId9" display="https://shellstorage123.blob.core.windows.net/portfoliopics/socialmedia/SM_Vid ("/>
+    <hyperlink ref="A2:A21" r:id="rId3" display="https://shellstorage123.blob.core.windows.net/cryptotracker/Crypto ("/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="66.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>